<commit_message>
script to download MODIS landcover
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="14880" windowHeight="8025" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="14880" windowHeight="8025" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Timeline" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="86">
   <si>
     <t>How much has C sink strength been reduced by the current drought?</t>
   </si>
@@ -193,14 +193,103 @@
   </si>
   <si>
     <t>metadata workflow, water data surface water, usgs</t>
+  </si>
+  <si>
+    <t>NCEAS Group Project - CA Drought</t>
+  </si>
+  <si>
+    <t>Timeline</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Lead</t>
+  </si>
+  <si>
+    <t>Help</t>
+  </si>
+  <si>
+    <t>Deadline</t>
+  </si>
+  <si>
+    <t>Friday presentation</t>
+  </si>
+  <si>
+    <t>Descriptive Analysis</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Paper</t>
+  </si>
+  <si>
+    <t>obtain flux data</t>
+  </si>
+  <si>
+    <t>obtain EVI</t>
+  </si>
+  <si>
+    <t>obtain LST</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>validate/test RECO</t>
+  </si>
+  <si>
+    <t>apply results spatially</t>
+  </si>
+  <si>
+    <t>Outline</t>
+  </si>
+  <si>
+    <t>Vicken</t>
+  </si>
+  <si>
+    <t>Deborah</t>
+  </si>
+  <si>
+    <t>Write</t>
+  </si>
+  <si>
+    <t>quantify changes by ecosystem type</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>PDSI x time</t>
+  </si>
+  <si>
+    <t>Runoff x time</t>
+  </si>
+  <si>
+    <t>Reservoir Storage x time</t>
+  </si>
+  <si>
+    <t>Cotton Yield x time</t>
+  </si>
+  <si>
+    <t>GPP x time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -216,7 +305,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -224,12 +313,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B10" sqref="A10:B10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,12 +972,191 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="33.5703125" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>41856</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="1">
+        <v>41859</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updates to task list
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="104">
   <si>
     <t>How much has C sink strength been reduced by the current drought?</t>
   </si>
@@ -207,9 +207,6 @@
     <t>Lead</t>
   </si>
   <si>
-    <t>Help</t>
-  </si>
-  <si>
     <t>Deadline</t>
   </si>
   <si>
@@ -228,12 +225,6 @@
     <t>obtain flux data</t>
   </si>
   <si>
-    <t>obtain EVI</t>
-  </si>
-  <si>
-    <t>obtain LST</t>
-  </si>
-  <si>
     <t>Paul</t>
   </si>
   <si>
@@ -249,18 +240,12 @@
     <t>Vicken</t>
   </si>
   <si>
-    <t>Deborah</t>
-  </si>
-  <si>
     <t>Write</t>
   </si>
   <si>
     <t>quantify changes by ecosystem type</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>PDSI x time</t>
   </si>
   <si>
@@ -274,6 +259,75 @@
   </si>
   <si>
     <t>GPP x time</t>
+  </si>
+  <si>
+    <t>obtain MODIS data</t>
+  </si>
+  <si>
+    <t>Figure help</t>
+  </si>
+  <si>
+    <t>Deborah?</t>
+  </si>
+  <si>
+    <t>Literature Review</t>
+  </si>
+  <si>
+    <t>Deborah, Mirela</t>
+  </si>
+  <si>
+    <t>Prep presentation</t>
+  </si>
+  <si>
+    <t>Detailed Review</t>
+  </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>Antonio, Sparkle</t>
+  </si>
+  <si>
+    <t>Vicken?</t>
+  </si>
+  <si>
+    <t>Leah?</t>
+  </si>
+  <si>
+    <t>Helpers</t>
   </si>
 </sst>
 </file>
@@ -297,12 +351,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -314,9 +386,15 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -326,11 +404,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -972,190 +1058,1029 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:AL25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" customWidth="1"/>
-    <col min="3" max="3" width="29.28515625" customWidth="1"/>
+    <col min="1" max="1" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="38" width="3.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>41856</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z5" s="6"/>
+      <c r="AA5" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB5" s="6"/>
+      <c r="AC5" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD5" s="6"/>
+      <c r="AE5" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="AF5" s="6"/>
+      <c r="AG5" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AH5" s="6"/>
+      <c r="AI5" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="AJ5" s="6"/>
+      <c r="AK5" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="AL5" s="6"/>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="4">
+        <v>41858</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="7"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="7"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="7"/>
+      <c r="AJ6" s="2"/>
+      <c r="AK6" s="7"/>
+      <c r="AL6" s="2"/>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="B7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="4">
+        <v>41859</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="7"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="7"/>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="7"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="7"/>
+      <c r="AJ7" s="2"/>
+      <c r="AK7" s="7"/>
+      <c r="AL7" s="2"/>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="2"/>
+      <c r="AJ8" s="2"/>
+      <c r="AK8" s="2"/>
+      <c r="AL8" s="2"/>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="1">
-        <v>41859</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="B9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+      <c r="AA9" s="2"/>
+      <c r="AB9" s="2"/>
+      <c r="AC9" s="2"/>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="2"/>
+      <c r="AH9" s="2"/>
+      <c r="AI9" s="2"/>
+      <c r="AJ9" s="2"/>
+      <c r="AK9" s="2"/>
+      <c r="AL9" s="2"/>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="B10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="2"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="2"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="2"/>
+      <c r="AB10" s="2"/>
+      <c r="AC10" s="2"/>
+      <c r="AD10" s="2"/>
+      <c r="AE10" s="2"/>
+      <c r="AF10" s="2"/>
+      <c r="AG10" s="2"/>
+      <c r="AH10" s="2"/>
+      <c r="AI10" s="2"/>
+      <c r="AJ10" s="2"/>
+      <c r="AK10" s="2"/>
+      <c r="AL10" s="2"/>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2"/>
+      <c r="AA11" s="2"/>
+      <c r="AB11" s="2"/>
+      <c r="AC11" s="2"/>
+      <c r="AD11" s="2"/>
+      <c r="AE11" s="2"/>
+      <c r="AF11" s="2"/>
+      <c r="AG11" s="2"/>
+      <c r="AH11" s="2"/>
+      <c r="AI11" s="2"/>
+      <c r="AJ11" s="2"/>
+      <c r="AK11" s="2"/>
+      <c r="AL11" s="2"/>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="2"/>
+      <c r="AB12" s="2"/>
+      <c r="AC12" s="2"/>
+      <c r="AD12" s="2"/>
+      <c r="AE12" s="2"/>
+      <c r="AF12" s="2"/>
+      <c r="AG12" s="2"/>
+      <c r="AH12" s="2"/>
+      <c r="AI12" s="2"/>
+      <c r="AJ12" s="2"/>
+      <c r="AK12" s="2"/>
+      <c r="AL12" s="2"/>
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2"/>
+      <c r="AA13" s="2"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="2"/>
+      <c r="AE13" s="2"/>
+      <c r="AF13" s="2"/>
+      <c r="AG13" s="2"/>
+      <c r="AH13" s="2"/>
+      <c r="AI13" s="2"/>
+      <c r="AJ13" s="2"/>
+      <c r="AK13" s="2"/>
+      <c r="AL13" s="2"/>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2"/>
+      <c r="AA14" s="2"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="2"/>
+      <c r="AD14" s="2"/>
+      <c r="AE14" s="2"/>
+      <c r="AF14" s="2"/>
+      <c r="AG14" s="2"/>
+      <c r="AH14" s="2"/>
+      <c r="AI14" s="2"/>
+      <c r="AJ14" s="2"/>
+      <c r="AK14" s="2"/>
+      <c r="AL14" s="2"/>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+      <c r="W15" s="2"/>
+      <c r="X15" s="2"/>
+      <c r="Y15" s="2"/>
+      <c r="Z15" s="2"/>
+      <c r="AA15" s="2"/>
+      <c r="AB15" s="2"/>
+      <c r="AC15" s="2"/>
+      <c r="AD15" s="2"/>
+      <c r="AE15" s="2"/>
+      <c r="AF15" s="2"/>
+      <c r="AG15" s="2"/>
+      <c r="AH15" s="2"/>
+      <c r="AI15" s="2"/>
+      <c r="AJ15" s="2"/>
+      <c r="AK15" s="2"/>
+      <c r="AL15" s="2"/>
+    </row>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="2"/>
+      <c r="AD16" s="2"/>
+      <c r="AE16" s="2"/>
+      <c r="AF16" s="2"/>
+      <c r="AG16" s="2"/>
+      <c r="AH16" s="2"/>
+      <c r="AI16" s="2"/>
+      <c r="AJ16" s="2"/>
+      <c r="AK16" s="2"/>
+      <c r="AL16" s="2"/>
+    </row>
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2"/>
+      <c r="Z17" s="2"/>
+      <c r="AA17" s="2"/>
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="2"/>
+      <c r="AD17" s="2"/>
+      <c r="AE17" s="2"/>
+      <c r="AF17" s="2"/>
+      <c r="AG17" s="2"/>
+      <c r="AH17" s="2"/>
+      <c r="AI17" s="2"/>
+      <c r="AJ17" s="2"/>
+      <c r="AK17" s="2"/>
+      <c r="AL17" s="2"/>
+    </row>
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="2"/>
+      <c r="AD18" s="2"/>
+      <c r="AE18" s="2"/>
+      <c r="AF18" s="2"/>
+      <c r="AG18" s="2"/>
+      <c r="AH18" s="2"/>
+      <c r="AI18" s="2"/>
+      <c r="AJ18" s="2"/>
+      <c r="AK18" s="2"/>
+      <c r="AL18" s="2"/>
+    </row>
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="2"/>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="2"/>
+      <c r="AD19" s="2"/>
+      <c r="AE19" s="2"/>
+      <c r="AF19" s="2"/>
+      <c r="AG19" s="2"/>
+      <c r="AH19" s="2"/>
+      <c r="AI19" s="2"/>
+      <c r="AJ19" s="2"/>
+      <c r="AK19" s="2"/>
+      <c r="AL19" s="2"/>
+    </row>
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="2"/>
+      <c r="Z20" s="2"/>
+      <c r="AA20" s="2"/>
+      <c r="AB20" s="2"/>
+      <c r="AC20" s="2"/>
+      <c r="AD20" s="2"/>
+      <c r="AE20" s="2"/>
+      <c r="AF20" s="2"/>
+      <c r="AG20" s="2"/>
+      <c r="AH20" s="2"/>
+      <c r="AI20" s="2"/>
+      <c r="AJ20" s="2"/>
+      <c r="AK20" s="2"/>
+      <c r="AL20" s="2"/>
+    </row>
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2"/>
+      <c r="Y21" s="2"/>
+      <c r="Z21" s="2"/>
+      <c r="AA21" s="2"/>
+      <c r="AB21" s="2"/>
+      <c r="AC21" s="2"/>
+      <c r="AD21" s="2"/>
+      <c r="AE21" s="2"/>
+      <c r="AF21" s="2"/>
+      <c r="AG21" s="2"/>
+      <c r="AH21" s="2"/>
+      <c r="AI21" s="2"/>
+      <c r="AJ21" s="2"/>
+      <c r="AK21" s="2"/>
+      <c r="AL21" s="2"/>
+    </row>
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="2"/>
+      <c r="Y22" s="2"/>
+      <c r="Z22" s="2"/>
+      <c r="AA22" s="2"/>
+      <c r="AB22" s="2"/>
+      <c r="AC22" s="2"/>
+      <c r="AD22" s="2"/>
+      <c r="AE22" s="2"/>
+      <c r="AF22" s="2"/>
+      <c r="AG22" s="2"/>
+      <c r="AH22" s="2"/>
+      <c r="AI22" s="2"/>
+      <c r="AJ22" s="2"/>
+      <c r="AK22" s="2"/>
+      <c r="AL22" s="2"/>
+    </row>
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="2"/>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2"/>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="2"/>
+      <c r="AD23" s="2"/>
+      <c r="AE23" s="2"/>
+      <c r="AF23" s="2"/>
+      <c r="AG23" s="2"/>
+      <c r="AH23" s="2"/>
+      <c r="AI23" s="2"/>
+      <c r="AJ23" s="2"/>
+      <c r="AK23" s="2"/>
+      <c r="AL23" s="2"/>
+    </row>
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B24" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>85</v>
-      </c>
-      <c r="B15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>69</v>
-      </c>
-      <c r="B23" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>70</v>
-      </c>
-      <c r="B24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>71</v>
-      </c>
-      <c r="B25" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>73</v>
-      </c>
-      <c r="B26" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>74</v>
-      </c>
-      <c r="B27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>79</v>
-      </c>
-      <c r="B28" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>75</v>
-      </c>
-      <c r="B33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>78</v>
-      </c>
-      <c r="B34" t="s">
-        <v>72</v>
-      </c>
-      <c r="C34" t="s">
-        <v>51</v>
-      </c>
+      <c r="C24" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2"/>
+      <c r="Y24" s="2"/>
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="2"/>
+      <c r="AB24" s="2"/>
+      <c r="AC24" s="2"/>
+      <c r="AD24" s="2"/>
+      <c r="AE24" s="2"/>
+      <c r="AF24" s="2"/>
+      <c r="AG24" s="2"/>
+      <c r="AH24" s="2"/>
+      <c r="AI24" s="2"/>
+      <c r="AJ24" s="2"/>
+      <c r="AK24" s="2"/>
+      <c r="AL24" s="2"/>
+    </row>
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="2"/>
+      <c r="Z25" s="2"/>
+      <c r="AA25" s="2"/>
+      <c r="AB25" s="2"/>
+      <c r="AC25" s="2"/>
+      <c r="AD25" s="2"/>
+      <c r="AE25" s="2"/>
+      <c r="AF25" s="2"/>
+      <c r="AG25" s="2"/>
+      <c r="AH25" s="2"/>
+      <c r="AI25" s="2"/>
+      <c r="AJ25" s="2"/>
+      <c r="AK25" s="2"/>
+      <c r="AL25" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AG5:AH5"/>
+    <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="E5:F5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
added outline for manuscript
</commit_message>
<xml_diff>
--- a/task.xlsx
+++ b/task.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="14840" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -757,16 +757,16 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
     <col min="2" max="2" width="78" customWidth="1"/>
-    <col min="3" max="3" width="62.5" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="8" max="8" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="62.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>8</v>
       </c>
@@ -777,7 +777,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -788,7 +788,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -796,17 +796,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -832,7 +832,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>39</v>
       </c>
@@ -846,7 +846,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>38</v>
       </c>
@@ -854,17 +854,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -878,7 +878,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>5</v>
       </c>
@@ -889,7 +889,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>2</v>
       </c>
@@ -900,7 +900,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>40</v>
       </c>
@@ -908,37 +908,37 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="2:2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="2:2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="2:2">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="2:2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="2:2">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="2:2">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>4</v>
       </c>
@@ -961,16 +961,16 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" customWidth="1"/>
-    <col min="3" max="3" width="6.5" customWidth="1"/>
-    <col min="4" max="4" width="7.33203125" customWidth="1"/>
-    <col min="5" max="5" width="7.5" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D1">
         <v>24</v>
       </c>
@@ -978,12 +978,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>28</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>55</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1103,34 +1103,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="38" width="3.33203125" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="38" width="3.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:38">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:38">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>41856</v>
       </c>
     </row>
-    <row r="5" spans="1:38">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>61</v>
       </c>
@@ -1212,7 +1212,7 @@
       </c>
       <c r="AL5" s="9"/>
     </row>
-    <row r="6" spans="1:38">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>86</v>
       </c>
@@ -1260,7 +1260,7 @@
       <c r="AK6" s="6"/>
       <c r="AL6" s="2"/>
     </row>
-    <row r="7" spans="1:38">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>64</v>
       </c>
@@ -1308,7 +1308,7 @@
       <c r="AK7" s="6"/>
       <c r="AL7" s="2"/>
     </row>
-    <row r="8" spans="1:38">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>65</v>
       </c>
@@ -1350,7 +1350,7 @@
       <c r="AK8" s="2"/>
       <c r="AL8" s="2"/>
     </row>
-    <row r="9" spans="1:38">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>76</v>
       </c>
@@ -1396,7 +1396,7 @@
       <c r="AK9" s="2"/>
       <c r="AL9" s="2"/>
     </row>
-    <row r="10" spans="1:38">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>77</v>
       </c>
@@ -1442,7 +1442,7 @@
       <c r="AK10" s="2"/>
       <c r="AL10" s="2"/>
     </row>
-    <row r="11" spans="1:38">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>78</v>
       </c>
@@ -1488,7 +1488,7 @@
       <c r="AK11" s="2"/>
       <c r="AL11" s="2"/>
     </row>
-    <row r="12" spans="1:38">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>79</v>
       </c>
@@ -1534,7 +1534,7 @@
       <c r="AK12" s="2"/>
       <c r="AL12" s="2"/>
     </row>
-    <row r="13" spans="1:38">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>80</v>
       </c>
@@ -1580,7 +1580,7 @@
       <c r="AK13" s="2"/>
       <c r="AL13" s="2"/>
     </row>
-    <row r="14" spans="1:38">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>66</v>
       </c>
@@ -1622,7 +1622,7 @@
       <c r="AK14" s="2"/>
       <c r="AL14" s="2"/>
     </row>
-    <row r="15" spans="1:38">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>68</v>
       </c>
@@ -1668,7 +1668,7 @@
       <c r="AK15" s="2"/>
       <c r="AL15" s="2"/>
     </row>
-    <row r="16" spans="1:38">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>81</v>
       </c>
@@ -1714,7 +1714,7 @@
       <c r="AK16" s="2"/>
       <c r="AL16" s="2"/>
     </row>
-    <row r="17" spans="1:38">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>70</v>
       </c>
@@ -1762,7 +1762,7 @@
       <c r="AK17" s="2"/>
       <c r="AL17" s="2"/>
     </row>
-    <row r="18" spans="1:38">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>71</v>
       </c>
@@ -1808,7 +1808,7 @@
       <c r="AK18" s="2"/>
       <c r="AL18" s="2"/>
     </row>
-    <row r="19" spans="1:38">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>75</v>
       </c>
@@ -1854,7 +1854,7 @@
       <c r="AK19" s="2"/>
       <c r="AL19" s="2"/>
     </row>
-    <row r="20" spans="1:38">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>67</v>
       </c>
@@ -1896,7 +1896,7 @@
       <c r="AK20" s="2"/>
       <c r="AL20" s="2"/>
     </row>
-    <row r="21" spans="1:38">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>72</v>
       </c>
@@ -1942,7 +1942,7 @@
       <c r="AK21" s="2"/>
       <c r="AL21" s="2"/>
     </row>
-    <row r="22" spans="1:38">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>84</v>
       </c>
@@ -1990,7 +1990,7 @@
       <c r="AK22" s="2"/>
       <c r="AL22" s="2"/>
     </row>
-    <row r="23" spans="1:38">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>87</v>
       </c>
@@ -2038,7 +2038,7 @@
       <c r="AK23" s="2"/>
       <c r="AL23" s="2"/>
     </row>
-    <row r="24" spans="1:38">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>74</v>
       </c>
@@ -2086,7 +2086,7 @@
       <c r="AK24" s="2"/>
       <c r="AL24" s="2"/>
     </row>
-    <row r="25" spans="1:38">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>82</v>
       </c>
@@ -2136,11 +2136,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="AK5:AL5"/>
     <mergeCell ref="Q5:R5"/>
@@ -2153,6 +2148,11 @@
     <mergeCell ref="AE5:AF5"/>
     <mergeCell ref="AG5:AH5"/>
     <mergeCell ref="AI5:AJ5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>